<commit_message>
Add results README and Weat 1-5 words
</commit_message>
<xml_diff>
--- a/reports/Results.xlsx
+++ b/reports/Results.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GRADSCHOOL\SemesterProjects\Navid\GitRepos\first-order-cooccurrence-metric-experiments\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C162B3C8-D5CE-436C-91E6-D6A6374C0DCF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3044127A-2FAE-49E2-AB63-F80E41C1FF27}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{7213AB31-3AB4-47A7-8AC4-F9A8CB97C1F2}"/>
+    <workbookView xWindow="-4640" yWindow="3040" windowWidth="10000" windowHeight="7460" xr2:uid="{7213AB31-3AB4-47A7-8AC4-F9A8CB97C1F2}"/>
   </bookViews>
   <sheets>
-    <sheet name="NavidGloVe" sheetId="3" r:id="rId1"/>
+    <sheet name="NavidWord2vec" sheetId="3" r:id="rId1"/>
     <sheet name="CaliskanGlove" sheetId="1" r:id="rId2"/>
     <sheet name="CaliskanWord2Vec" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="9">
   <si>
     <t>2nd order</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>1st order</t>
+  </si>
+  <si>
+    <t>WEAT 10</t>
+  </si>
+  <si>
+    <t>WEAT 5</t>
   </si>
 </sst>
 </file>
@@ -405,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A402D8-3C1F-4C2D-B87E-B11158E9EC84}">
-  <dimension ref="A2:E6"/>
+  <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -437,44 +443,72 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>1.774</v>
+        <v>0.72</v>
       </c>
       <c r="C4">
-        <v>1.95E-4</v>
+        <v>0.01</v>
       </c>
       <c r="D4">
-        <v>1.8160000000000001</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>1.595</v>
+        <v>1.774</v>
       </c>
       <c r="C5">
-        <v>7.1000000000000002E-4</v>
+        <v>1.95E-4</v>
       </c>
       <c r="D5">
-        <v>1.647</v>
+        <v>1.8160000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1.595</v>
+      </c>
+      <c r="C6">
+        <v>7.1000000000000002E-4</v>
+      </c>
+      <c r="D6">
+        <v>1.647</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>1.4179999999999999</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>2.2799999999999999E-3</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>1.4710000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-0.08</v>
+      </c>
+      <c r="C8">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D8">
+        <v>-0.318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>